<commit_message>
Initial draft of the PM2.5 (sat vs. obs) comparison
</commit_message>
<xml_diff>
--- a/sunny_VK_LB.xlsx
+++ b/sunny_VK_LB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Variable</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Q*</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>No</t>
@@ -431,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +492,10 @@
         <v>0.0443967897429744</v>
       </c>
       <c r="H2">
-        <v>0.9646803868489953</v>
+        <v>0.9646803381026858</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -518,10 +521,10 @@
         <v>3.001141525128701</v>
       </c>
       <c r="H3">
-        <v>0.003694659525422797</v>
+        <v>0.003427539896620487</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -544,13 +547,13 @@
         <v>0.9673146984423985</v>
       </c>
       <c r="G4">
-        <v>0.09289560375421289</v>
+        <v>0.09289560375421288</v>
       </c>
       <c r="H4">
-        <v>0.9261843813677169</v>
+        <v>0.9261800894161204</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -576,10 +579,10 @@
         <v>-0.3450086890792463</v>
       </c>
       <c r="H5">
-        <v>0.7309262751326332</v>
+        <v>0.7308425919715824</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -605,10 +608,10 @@
         <v>-0.4511078622858415</v>
       </c>
       <c r="H6">
-        <v>0.652949443319366</v>
+        <v>0.6529291562813258</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -631,13 +634,13 @@
         <v>0.8495658428595478</v>
       </c>
       <c r="G7">
-        <v>-3.810620297534497</v>
+        <v>-3.810620297534498</v>
       </c>
       <c r="H7">
-        <v>0.0003345852307494238</v>
+        <v>0.0002446487635881599</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -663,10 +666,10 @@
         <v>3.90637159075347</v>
       </c>
       <c r="H8">
-        <v>0.0002228703049041837</v>
+        <v>0.0001743429192672115</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -692,10 +695,10 @@
         <v>1.156008955631869</v>
       </c>
       <c r="H9">
-        <v>0.2529582888336905</v>
+        <v>0.2505463453197566</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -721,10 +724,39 @@
         <v>0.69655185931271</v>
       </c>
       <c r="H10">
-        <v>0.4878101308289806</v>
+        <v>0.4877664561713912</v>
       </c>
       <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
         <v>18</v>
+      </c>
+      <c r="B11">
+        <v>-0.5685414527331637</v>
+      </c>
+      <c r="C11">
+        <v>-2.810999543124124</v>
+      </c>
+      <c r="D11">
+        <v>0.7609251830041186</v>
+      </c>
+      <c r="E11">
+        <v>17.17363614673463</v>
+      </c>
+      <c r="F11">
+        <v>0.2964689350684678</v>
+      </c>
+      <c r="G11">
+        <v>0.9131334187456903</v>
+      </c>
+      <c r="H11">
+        <v>0.3634599521358221</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>